<commit_message>
Update Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
Agregue 4 tablas mas cambie un poco la de codigo postal
</commit_message>
<xml_diff>
--- a/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
+++ b/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Ramos\Desktop\repositorio de github\proyecto_de_bases1_spotify\Modelo_de_base_de_datos\modelo Entidad-Relacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\GitHub\proyecto_de_bases1_spotify\Modelo_de_base_de_datos\modelo Entidad-Relacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>Codigo usuario</t>
   </si>
@@ -125,9 +125,6 @@
     <t>EEUU</t>
   </si>
   <si>
-    <t>Codigo Postal</t>
-  </si>
-  <si>
     <t>Numero codigo postal</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>Android</t>
   </si>
   <si>
-    <t>Symbian</t>
-  </si>
-  <si>
     <t xml:space="preserve">Windows mobile </t>
   </si>
   <si>
@@ -207,13 +201,73 @@
   </si>
   <si>
     <t>Verizon</t>
+  </si>
+  <si>
+    <t>Codigo Pais de Proveedor movil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo Pais </t>
+  </si>
+  <si>
+    <t>Codigo Proveedor</t>
+  </si>
+  <si>
+    <t>AT&amp;T</t>
+  </si>
+  <si>
+    <t>Nombre Sistema Operativo</t>
+  </si>
+  <si>
+    <t>Codigo Sistema Operativo</t>
+  </si>
+  <si>
+    <t>Mac Os</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Sistemas Operativo de moviles</t>
+  </si>
+  <si>
+    <t>Black Berry OS</t>
+  </si>
+  <si>
+    <t>Sistema Operativo por marca</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>Codigo Postal x pais</t>
+  </si>
+  <si>
+    <t>Codigo postal</t>
+  </si>
+  <si>
+    <t>Nombre de la region</t>
+  </si>
+  <si>
+    <t>Francisco Morazan</t>
+  </si>
+  <si>
+    <t>EL paraiso</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Carolina del norte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,16 +290,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -277,12 +351,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -292,14 +463,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,7 +568,7 @@
   </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" name="Codigo pais"/>
-    <tableColumn id="2" name="Numero codigo postal"/>
+    <tableColumn id="2" name="Codigo postal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -419,8 +603,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J12:K15" totalsRowShown="0">
-  <autoFilter ref="J12:K15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J12:K16" totalsRowShown="0">
+  <autoFilter ref="J12:K16">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
@@ -433,7 +617,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -695,36 +879,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z22"/>
+  <dimension ref="B2:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
@@ -742,10 +926,10 @@
         <v>25</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,16 +955,16 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
         <v>41</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>42</v>
-      </c>
-      <c r="M3" t="s">
-        <v>43</v>
       </c>
       <c r="Q3" t="s">
         <v>6</v>
@@ -798,10 +982,10 @@
         <v>26</v>
       </c>
       <c r="Z3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -854,10 +1038,10 @@
         <v>1</v>
       </c>
       <c r="Z4">
-        <v>11101</v>
-      </c>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -910,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="Z5" s="8">
-        <v>13201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -960,10 +1144,10 @@
         <v>5</v>
       </c>
       <c r="Z6">
-        <v>33109</v>
-      </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U7">
         <v>4</v>
       </c>
@@ -974,10 +1158,10 @@
         <v>5</v>
       </c>
       <c r="Z7">
-        <v>28459</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U8">
         <v>5</v>
       </c>
@@ -985,103 +1169,190 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA12" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="M13" s="10">
+        <v>1</v>
+      </c>
+      <c r="N13" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="11">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="19">
+        <v>11101</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-      <c r="K14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="20">
+        <v>13201</v>
+      </c>
+      <c r="AA14" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="M15" s="11">
+        <v>5</v>
+      </c>
+      <c r="N15" s="11">
+        <v>3</v>
+      </c>
+      <c r="Y15" s="11">
+        <v>3</v>
+      </c>
+      <c r="Z15" s="19">
+        <v>33109</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="14">
+        <v>5</v>
+      </c>
+      <c r="N16" s="14">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="7">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="21">
+        <v>28459</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">
@@ -1089,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.25">
@@ -1097,7 +1368,7 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.25">
@@ -1105,7 +1376,7 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.25">
@@ -1113,7 +1384,7 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.25">
@@ -1121,7 +1392,7 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.25">
@@ -1129,7 +1400,145 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="11">
+        <v>2</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="7">
+        <v>3</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" s="11">
+        <v>4</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" s="11">
+        <v>1</v>
+      </c>
+      <c r="G34" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="11">
+        <v>3</v>
+      </c>
+      <c r="G36" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38" s="11">
+        <v>4</v>
+      </c>
+      <c r="G38" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="11">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="11">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="7">
+        <v>2</v>
+      </c>
+      <c r="G43" s="7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avance de trabajo de modelo de basa de datos
</commit_message>
<xml_diff>
--- a/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
+++ b/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
   <si>
     <t>Codigo usuario</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Femenino</t>
   </si>
   <si>
-    <t>Pais</t>
-  </si>
-  <si>
     <t>Codigo pais</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Honduras</t>
   </si>
   <si>
-    <t>El salvador</t>
-  </si>
-  <si>
     <t>Guatemala</t>
   </si>
   <si>
@@ -200,51 +194,30 @@
     <t>Claro</t>
   </si>
   <si>
-    <t>Verizon</t>
-  </si>
-  <si>
-    <t>Codigo Pais de Proveedor movil</t>
-  </si>
-  <si>
     <t xml:space="preserve">Codigo Pais </t>
   </si>
   <si>
     <t>Codigo Proveedor</t>
   </si>
   <si>
-    <t>AT&amp;T</t>
-  </si>
-  <si>
     <t>Nombre Sistema Operativo</t>
   </si>
   <si>
     <t>Codigo Sistema Operativo</t>
   </si>
   <si>
-    <t>Mac Os</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>Sistemas Operativo de moviles</t>
   </si>
   <si>
     <t>Black Berry OS</t>
   </si>
   <si>
-    <t>Sistema Operativo por marca</t>
-  </si>
-  <si>
     <t>HTC</t>
   </si>
   <si>
     <t>Lenovo</t>
   </si>
   <si>
-    <t>Codigo Postal x pais</t>
-  </si>
-  <si>
     <t>Codigo postal</t>
   </si>
   <si>
@@ -261,6 +234,123 @@
   </si>
   <si>
     <t>Carolina del norte</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Sistema Operativo x Marca de telefono movil</t>
+  </si>
+  <si>
+    <t>symbian OS</t>
+  </si>
+  <si>
+    <t>Windows Phone</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>proveedores de servicio movil x pais</t>
+  </si>
+  <si>
+    <t>Generos musicales</t>
+  </si>
+  <si>
+    <t>Nombre del genero</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Bachata</t>
+  </si>
+  <si>
+    <t>Hip Hop</t>
+  </si>
+  <si>
+    <t>Ranchera</t>
+  </si>
+  <si>
+    <t>Merengue</t>
+  </si>
+  <si>
+    <t>Rap</t>
+  </si>
+  <si>
+    <t>Electronica</t>
+  </si>
+  <si>
+    <t>Reggaeton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Generos musicales x Ususario</t>
+  </si>
+  <si>
+    <t>Codigo de genero</t>
+  </si>
+  <si>
+    <t>Codigo de usuario</t>
+  </si>
+  <si>
+    <t>Fecha que selecciono genero</t>
+  </si>
+  <si>
+    <t>Rock alternativo</t>
+  </si>
+  <si>
+    <t>Grupos musicales o artistas</t>
+  </si>
+  <si>
+    <t>Nombre de grupo musical o artista</t>
+  </si>
+  <si>
+    <t>Codigo de grupo musical o artista</t>
+  </si>
+  <si>
+    <t>Codigo album</t>
+  </si>
+  <si>
+    <t>codigo pais</t>
+  </si>
+  <si>
+    <t>Paises</t>
+  </si>
+  <si>
+    <t>Linkin park</t>
+  </si>
+  <si>
+    <t>Madona</t>
+  </si>
+  <si>
+    <t>Vicente Fernandes</t>
+  </si>
+  <si>
+    <t>Polache</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Albunes musicales</t>
+  </si>
+  <si>
+    <t>Nombre album</t>
+  </si>
+  <si>
+    <t>Canciones</t>
+  </si>
+  <si>
+    <t>Codigo cancion</t>
+  </si>
+  <si>
+    <t>Nombre de la cancion</t>
   </si>
 </sst>
 </file>
@@ -319,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -446,12 +536,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -460,7 +563,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -474,12 +576,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -515,7 +639,7 @@
   <tableColumns count="12">
     <tableColumn id="1" name="Codigo usuario"/>
     <tableColumn id="2" name="Nombre completo"/>
-    <tableColumn id="3" name="Fecha de nacimiento" dataDxfId="0"/>
+    <tableColumn id="3" name="Fecha de nacimiento" dataDxfId="2"/>
     <tableColumn id="4" name="Codigo Genero"/>
     <tableColumn id="5" name="Usuario de platafoma"/>
     <tableColumn id="6" name="Correo electonico"/>
@@ -525,6 +649,54 @@
     <tableColumn id="10" name="Numero de telefono"/>
     <tableColumn id="11" name="Codigo Marca de telefono movil"/>
     <tableColumn id="12" name="Codigo Proveedor de servicio movil"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="J36:N40" totalsRowShown="0">
+  <autoFilter ref="J36:N40">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Codigo de grupo musical o artista"/>
+    <tableColumn id="2" name="Nombre de grupo musical o artista"/>
+    <tableColumn id="3" name="codigo pais"/>
+    <tableColumn id="4" name="Codigo album"/>
+    <tableColumn id="5" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="J44:K47" totalsRowShown="0">
+  <autoFilter ref="J44:K47">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo album"/>
+    <tableColumn id="2" name="Nombre album"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="J54:K57" totalsRowShown="0">
+  <autoFilter ref="J54:K57">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo cancion"/>
+    <tableColumn id="2" name="Nombre de la cancion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -559,20 +731,6 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="Y3:Z7" totalsRowShown="0">
-  <autoFilter ref="Y3:Z7">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Codigo pais"/>
-    <tableColumn id="2" name="Codigo postal"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B12:C15" totalsRowShown="0">
   <autoFilter ref="B12:C15">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -586,7 +744,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="F12:G22" totalsRowShown="0">
   <autoFilter ref="F12:G22">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -600,15 +758,63 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J12:K16" totalsRowShown="0">
-  <autoFilter ref="J12:K16">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="U21:V23" totalsRowShown="0">
+  <autoFilter ref="U21:V23">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" name="Codigo Proveedor de servicio movil"/>
     <tableColumn id="2" name="Nombre del proveedor"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="Y3:AB7" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="Y3:AB7">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Codigo postal"/>
+    <tableColumn id="2" name="Codigo pais"/>
+    <tableColumn id="3" name="Numero codigo postal"/>
+    <tableColumn id="4" name="Nombre de la region"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="J12:L22" totalsRowShown="0">
+  <autoFilter ref="J12:L22">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Codigo de genero"/>
+    <tableColumn id="2" name="Nombre del genero"/>
+    <tableColumn id="3" name="Fecha que selecciono genero"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="J26:K31" totalsRowShown="0">
+  <autoFilter ref="J26:K31">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo de genero"/>
+    <tableColumn id="2" name="Codigo de usuario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -877,37 +1083,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AA43"/>
+  <dimension ref="B2:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" customWidth="1"/>
+    <col min="11" max="11" width="41.5703125" customWidth="1"/>
+    <col min="12" max="12" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
@@ -922,13 +1132,13 @@
         <v>21</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,16 +1164,16 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" t="s">
-        <v>42</v>
       </c>
       <c r="Q3" t="s">
         <v>6</v>
@@ -972,19 +1182,25 @@
         <v>22</v>
       </c>
       <c r="U3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" t="s">
         <v>26</v>
       </c>
-      <c r="V3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>26</v>
+      <c r="Y3" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="Z3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1031,16 +1247,22 @@
         <v>1</v>
       </c>
       <c r="V4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y4">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="22">
         <v>1</v>
       </c>
       <c r="Z4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AA4" s="17">
+        <v>11101</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1087,16 +1309,22 @@
         <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="8">
+        <v>103</v>
+      </c>
+      <c r="Y5" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="18">
+        <v>13201</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -1137,407 +1365,554 @@
         <v>3</v>
       </c>
       <c r="V6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y6">
+        <v>28</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>3</v>
+      </c>
+      <c r="Z6">
         <v>5</v>
       </c>
-      <c r="Z6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AA6" s="17">
+        <v>33109</v>
+      </c>
+      <c r="AB6" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="U7">
         <v>4</v>
       </c>
       <c r="V7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y7">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="21">
+        <v>4</v>
+      </c>
+      <c r="Z7">
         <v>5</v>
       </c>
-      <c r="Z7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AA7" s="19">
+        <v>28459</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="U8">
         <v>5</v>
       </c>
       <c r="V8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" t="s">
+        <v>91</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y11" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA12" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
-      </c>
-      <c r="M13" s="10">
-        <v>1</v>
-      </c>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="18">
-        <v>11101</v>
-      </c>
-      <c r="AA13" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="L13" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U13" s="9">
+        <v>1</v>
+      </c>
+      <c r="V13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="7">
-        <v>1</v>
-      </c>
-      <c r="N14" s="7">
+        <v>79</v>
+      </c>
+      <c r="L14" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U14" s="7">
+        <v>1</v>
+      </c>
+      <c r="V14" s="7">
         <v>2</v>
       </c>
-      <c r="Y14" s="7">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="19">
-        <v>13201</v>
-      </c>
-      <c r="AA14" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
-      </c>
-      <c r="M15" s="11">
-        <v>5</v>
-      </c>
-      <c r="N15" s="11">
-        <v>3</v>
-      </c>
-      <c r="Y15" s="11">
-        <v>3</v>
-      </c>
-      <c r="Z15" s="18">
-        <v>33109</v>
-      </c>
-      <c r="AA15" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L15" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U15" s="10">
+        <v>2</v>
+      </c>
+      <c r="V15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J16">
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
-      </c>
-      <c r="M16" s="14">
-        <v>5</v>
-      </c>
-      <c r="N16" s="14">
+        <v>81</v>
+      </c>
+      <c r="L16" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U16" s="13">
         <v>4</v>
       </c>
-      <c r="Y16" s="7">
-        <v>4</v>
-      </c>
-      <c r="Z16" s="20">
-        <v>28459</v>
-      </c>
-      <c r="AA16" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="V16" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" s="23">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="23">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="J19">
+        <v>7</v>
+      </c>
+      <c r="K19" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="23">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="K21" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U21" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="15" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>86</v>
+      </c>
+      <c r="L22" s="23">
+        <v>41255</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="V23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F26" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="9">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="11">
+        <v>39</v>
+      </c>
+      <c r="J26" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="10">
+        <v>3</v>
+      </c>
+      <c r="G29" s="10">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F30" s="7">
         <v>2</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="7">
+      <c r="G30" s="7">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>8</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F31" s="10">
+        <v>4</v>
+      </c>
+      <c r="G31" s="10">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+      <c r="K31">
         <v>3</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="11">
+    </row>
+    <row r="34" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F36" s="8">
+        <v>1</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" t="s">
+        <v>94</v>
+      </c>
+      <c r="L36" t="s">
+        <v>97</v>
+      </c>
+      <c r="M36" t="s">
+        <v>96</v>
+      </c>
+      <c r="N36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F37" s="10">
+        <v>2</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>99</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F38" s="7">
+        <v>3</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38" t="s">
+        <v>100</v>
+      </c>
+      <c r="L38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F39" s="10">
         <v>4</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F32" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F34" s="11">
-        <v>1</v>
-      </c>
-      <c r="G34" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F35" s="7">
-        <v>1</v>
-      </c>
-      <c r="G35" s="7">
+      <c r="G39" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>102</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F40" s="7">
+        <v>5</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40" t="s">
+        <v>101</v>
+      </c>
+      <c r="L40">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F36" s="11">
-        <v>3</v>
-      </c>
-      <c r="G36" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="7">
-        <v>2</v>
-      </c>
-      <c r="G37" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="11">
-        <v>4</v>
-      </c>
-      <c r="G38" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F39" s="7">
-        <v>1</v>
-      </c>
-      <c r="G39" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F40" s="11">
-        <v>1</v>
-      </c>
-      <c r="G40" s="11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="11">
-        <v>1</v>
-      </c>
-      <c r="G42" s="11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F43" s="7">
-        <v>2</v>
-      </c>
-      <c r="G43" s="7">
-        <v>10</v>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="J43" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>96</v>
+      </c>
+      <c r="K44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1923,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
-  <tableParts count="7">
+  <tableParts count="12">
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
@@ -1556,6 +1931,11 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creacion de nuevas tablas para canciones, albunes, y artistas
</commit_message>
<xml_diff>
--- a/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
+++ b/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
   <si>
     <t>Codigo usuario</t>
   </si>
@@ -119,9 +119,6 @@
     <t>EEUU</t>
   </si>
   <si>
-    <t>Numero codigo postal</t>
-  </si>
-  <si>
     <t>Codigo tipo de plan</t>
   </si>
   <si>
@@ -218,27 +215,9 @@
     <t>Lenovo</t>
   </si>
   <si>
-    <t>Codigo postal</t>
-  </si>
-  <si>
-    <t>Nombre de la region</t>
-  </si>
-  <si>
     <t>Francisco Morazan</t>
   </si>
   <si>
-    <t>EL paraiso</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Carolina del norte</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Sistema Operativo x Marca de telefono movil</t>
   </si>
   <si>
@@ -293,15 +272,9 @@
     <t>Generos musicales x Ususario</t>
   </si>
   <si>
-    <t>Codigo de genero</t>
-  </si>
-  <si>
     <t>Codigo de usuario</t>
   </si>
   <si>
-    <t>Fecha que selecciono genero</t>
-  </si>
-  <si>
     <t>Rock alternativo</t>
   </si>
   <si>
@@ -351,13 +324,169 @@
   </si>
   <si>
     <t>Nombre de la cancion</t>
+  </si>
+  <si>
+    <t>Nombre de la ciudad</t>
+  </si>
+  <si>
+    <t>Codigo ciudad</t>
+  </si>
+  <si>
+    <t>codigo de codigo postal</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Codigo departamento</t>
+  </si>
+  <si>
+    <t>Nombre del departamento</t>
+  </si>
+  <si>
+    <t>Tegucigalpa</t>
+  </si>
+  <si>
+    <t>La Ceiba</t>
+  </si>
+  <si>
+    <t>Atlantida</t>
+  </si>
+  <si>
+    <t>dep. De guatemala</t>
+  </si>
+  <si>
+    <t>León</t>
+  </si>
+  <si>
+    <t>La Paz Centro</t>
+  </si>
+  <si>
+    <t>SAN PEDRO AYAMPUC</t>
+  </si>
+  <si>
+    <t>No body can save me</t>
+  </si>
+  <si>
+    <t>duracion de la cancion</t>
+  </si>
+  <si>
+    <t>Genero de cancion</t>
+  </si>
+  <si>
+    <t>Grupo musical o artista</t>
+  </si>
+  <si>
+    <t>album musical</t>
+  </si>
+  <si>
+    <t>Numero de me gusta</t>
+  </si>
+  <si>
+    <t>One more light</t>
+  </si>
+  <si>
+    <t>Give me all your luvin'</t>
+  </si>
+  <si>
+    <t>Segidores</t>
+  </si>
+  <si>
+    <t>Biografia</t>
+  </si>
+  <si>
+    <t>Reportes recibidos</t>
+  </si>
+  <si>
+    <t>Numero de shares</t>
+  </si>
+  <si>
+    <t>Conciertos</t>
+  </si>
+  <si>
+    <t>Play list</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>codigo de play list</t>
+  </si>
+  <si>
+    <t>Nombre de play list</t>
+  </si>
+  <si>
+    <t>Estado de play list</t>
+  </si>
+  <si>
+    <t>Codigo Usuario</t>
+  </si>
+  <si>
+    <t>Privado</t>
+  </si>
+  <si>
+    <t>Publica</t>
+  </si>
+  <si>
+    <t>bachata</t>
+  </si>
+  <si>
+    <t>Tiempo escuchado</t>
+  </si>
+  <si>
+    <t>Codigo Grupos musicales o artistas</t>
+  </si>
+  <si>
+    <t>Fecha en que escucho el artista</t>
+  </si>
+  <si>
+    <t>Grupos musicales o artistas X usuario</t>
+  </si>
+  <si>
+    <t>Codigo de genero musical</t>
+  </si>
+  <si>
+    <t>Codigo genero musical</t>
+  </si>
+  <si>
+    <t>Generos musicales X grupos musicales o artistas</t>
+  </si>
+  <si>
+    <t>Fecha que se anadio genero</t>
+  </si>
+  <si>
+    <t>Fecha en que anade genero a su cuenta</t>
+  </si>
+  <si>
+    <t>La potra</t>
+  </si>
+  <si>
+    <t>Ms romantico que nunca</t>
+  </si>
+  <si>
+    <t>Numero de canciones</t>
+  </si>
+  <si>
+    <t>duracion de album</t>
+  </si>
+  <si>
+    <t>Fecha de creacion</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>hip hop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,8 +517,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF005297"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,8 +549,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -549,12 +696,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -574,17 +747,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -595,13 +782,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
       </border>
     </dxf>
     <dxf>
@@ -655,48 +835,152 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="J36:N40" totalsRowShown="0">
-  <autoFilter ref="J36:N40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="J36:R40" totalsRowShown="0">
+  <autoFilter ref="J36:R40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="5">
+  <tableColumns count="9">
     <tableColumn id="1" name="Codigo de grupo musical o artista"/>
     <tableColumn id="2" name="Nombre de grupo musical o artista"/>
     <tableColumn id="3" name="codigo pais"/>
-    <tableColumn id="4" name="Codigo album"/>
-    <tableColumn id="5" name="Column1"/>
+    <tableColumn id="5" name="Segidores"/>
+    <tableColumn id="7" name="Biografia"/>
+    <tableColumn id="8" name="Reportes recibidos"/>
+    <tableColumn id="9" name="Numero de shares"/>
+    <tableColumn id="10" name="Conciertos"/>
+    <tableColumn id="11" name="Radio"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="J44:K47" totalsRowShown="0">
-  <autoFilter ref="J44:K47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="J44:O48" totalsRowShown="0">
+  <autoFilter ref="J44:O48">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
+  <tableColumns count="6">
     <tableColumn id="1" name="Codigo album"/>
     <tableColumn id="2" name="Nombre album"/>
+    <tableColumn id="3" name="Numero de canciones"/>
+    <tableColumn id="4" name="duracion de album"/>
+    <tableColumn id="5" name="Fecha de creacion"/>
+    <tableColumn id="6" name="Codigo de grupo musical o artista"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="J54:K57" totalsRowShown="0">
-  <autoFilter ref="J54:K57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="J54:P57" totalsRowShown="0">
+  <autoFilter ref="J54:P57">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Codigo cancion"/>
+    <tableColumn id="2" name="Nombre de la cancion"/>
+    <tableColumn id="3" name="duracion de la cancion"/>
+    <tableColumn id="5" name="Genero de cancion"/>
+    <tableColumn id="6" name="Grupo musical o artista"/>
+    <tableColumn id="7" name="album musical"/>
+    <tableColumn id="8" name="Numero de me gusta"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="Y12:AA16" totalsRowShown="0">
+  <autoFilter ref="Y12:AA16">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Codigo departamento"/>
+    <tableColumn id="2" name="Nombre del departamento"/>
+    <tableColumn id="3" name="Codigo pais"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="J63:M66" totalsRowShown="0">
+  <autoFilter ref="J63:M66">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" name="codigo de play list"/>
+    <tableColumn id="2" name="Nombre de play list"/>
+    <tableColumn id="3" name="Estado de play list"/>
+    <tableColumn id="4" name="Codigo Usuario"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="L72:N75" totalsRowShown="0">
+  <autoFilter ref="L72:N75">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="3" name="Codigo genero musical"/>
+    <tableColumn id="4" name="Tiempo escuchado"/>
+    <tableColumn id="5" name="Fecha en que escucho el artista"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="J72:K75" totalsRowShown="0">
+  <autoFilter ref="J72:K75">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Codigo cancion"/>
-    <tableColumn id="2" name="Nombre de la cancion"/>
+    <tableColumn id="1" name="Codigo Grupos musicales o artistas"/>
+    <tableColumn id="2" name="Codigo usuario"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="N26:O29" totalsRowShown="0">
+  <autoFilter ref="N26:O29">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo de genero musical"/>
+    <tableColumn id="2" name="Codigo de grupo musical o artista"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,7 +1057,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="Y3:AB7" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="Y3:AB7" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="Y3:AB7">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -781,10 +1065,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Codigo postal"/>
-    <tableColumn id="2" name="Codigo pais"/>
-    <tableColumn id="3" name="Numero codigo postal"/>
-    <tableColumn id="4" name="Nombre de la region"/>
+    <tableColumn id="1" name="Codigo ciudad"/>
+    <tableColumn id="2" name="Nombre de la ciudad"/>
+    <tableColumn id="3" name="codigo de codigo postal"/>
+    <tableColumn id="4" name="Codigo departamento"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -798,23 +1082,25 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="Codigo de genero"/>
+    <tableColumn id="1" name="Codigo de genero musical"/>
     <tableColumn id="2" name="Nombre del genero"/>
-    <tableColumn id="3" name="Fecha que selecciono genero"/>
+    <tableColumn id="3" name="Fecha que se anadio genero"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="J26:K31" totalsRowShown="0">
-  <autoFilter ref="J26:K31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="J26:L31" totalsRowShown="0">
+  <autoFilter ref="J26:L31">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Codigo de genero"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Codigo de genero musical"/>
     <tableColumn id="2" name="Codigo de usuario"/>
+    <tableColumn id="3" name="Fecha en que anade genero a su cuenta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1083,37 +1369,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AB54"/>
+  <dimension ref="B2:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="41" customWidth="1"/>
     <col min="11" max="11" width="41.5703125" customWidth="1"/>
-    <col min="12" max="12" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.7109375" customWidth="1"/>
+    <col min="26" max="26" width="32.42578125" customWidth="1"/>
+    <col min="27" max="27" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1132,10 +1418,10 @@
         <v>21</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
@@ -1164,16 +1450,16 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>39</v>
-      </c>
-      <c r="M3" t="s">
-        <v>40</v>
       </c>
       <c r="Q3" t="s">
         <v>6</v>
@@ -1187,17 +1473,17 @@
       <c r="V3" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="21" t="s">
-        <v>64</v>
+      <c r="Y3" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="Z3" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>65</v>
+        <v>102</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
@@ -1249,20 +1535,20 @@
       <c r="V4" t="s">
         <v>27</v>
       </c>
-      <c r="Y4" s="22">
-        <v>1</v>
-      </c>
-      <c r="Z4">
-        <v>1</v>
+      <c r="Y4" s="21">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>107</v>
       </c>
       <c r="AA4" s="17">
         <v>11101</v>
       </c>
-      <c r="AB4" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AB4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1309,22 +1595,22 @@
         <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y5" s="21">
-        <v>2</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>108</v>
       </c>
       <c r="AA5" s="18">
-        <v>13201</v>
-      </c>
-      <c r="AB5" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+        <v>31101</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -1367,37 +1653,37 @@
       <c r="V6" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="22">
+      <c r="Y6" s="21">
         <v>3</v>
       </c>
-      <c r="Z6">
-        <v>5</v>
-      </c>
-      <c r="AA6" s="17">
-        <v>33109</v>
-      </c>
-      <c r="AB6" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="Z6" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA6" s="24">
+        <v>22100</v>
+      </c>
+      <c r="AB6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" ht="16.5" x14ac:dyDescent="0.3">
       <c r="U7">
         <v>4</v>
       </c>
       <c r="V7" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="Y7" s="20">
         <v>4</v>
       </c>
-      <c r="Z7">
-        <v>5</v>
-      </c>
-      <c r="AA7" s="19">
-        <v>28459</v>
-      </c>
-      <c r="AB7" s="7" t="s">
-        <v>69</v>
+      <c r="Z7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>1056</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
@@ -1410,45 +1696,57 @@
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="Y11" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="K12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="U12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="V12" s="12" t="s">
-        <v>57</v>
+      <c r="Y12" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
@@ -1456,27 +1754,36 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="23">
+        <v>71</v>
+      </c>
+      <c r="L13" s="22">
         <v>41255</v>
       </c>
       <c r="U13" s="9">
         <v>1</v>
       </c>
       <c r="V13" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA13">
         <v>1</v>
       </c>
     </row>
@@ -1485,21 +1792,21 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="23">
+        <v>72</v>
+      </c>
+      <c r="L14" s="22">
         <v>41255</v>
       </c>
       <c r="U14" s="7">
@@ -1507,6 +1814,15 @@
       </c>
       <c r="V14" s="7">
         <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
@@ -1514,21 +1830,21 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="23">
+        <v>73</v>
+      </c>
+      <c r="L15" s="22">
         <v>41255</v>
       </c>
       <c r="U15" s="10">
@@ -1536,6 +1852,15 @@
       </c>
       <c r="V15" s="10">
         <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>3</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
@@ -1543,15 +1868,15 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16">
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>81</v>
-      </c>
-      <c r="L16" s="23">
+        <v>74</v>
+      </c>
+      <c r="L16" s="22">
         <v>41255</v>
       </c>
       <c r="U16" s="13">
@@ -1559,6 +1884,15 @@
       </c>
       <c r="V16" s="13">
         <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA16">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="6:22" x14ac:dyDescent="0.25">
@@ -1566,15 +1900,15 @@
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17">
         <v>5</v>
       </c>
       <c r="K17" t="s">
-        <v>82</v>
-      </c>
-      <c r="L17" s="23">
+        <v>75</v>
+      </c>
+      <c r="L17" s="22">
         <v>41255</v>
       </c>
     </row>
@@ -1583,15 +1917,15 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18">
         <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18" s="23">
+        <v>83</v>
+      </c>
+      <c r="L18" s="22">
         <v>41255</v>
       </c>
     </row>
@@ -1600,15 +1934,15 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J19">
         <v>7</v>
       </c>
       <c r="K19" t="s">
-        <v>83</v>
-      </c>
-      <c r="L19" s="23">
+        <v>76</v>
+      </c>
+      <c r="L19" s="22">
         <v>41255</v>
       </c>
     </row>
@@ -1617,19 +1951,19 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J20">
         <v>8</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L20" s="23">
+        <v>77</v>
+      </c>
+      <c r="L20" s="22">
         <v>41255</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="6:22" x14ac:dyDescent="0.25">
@@ -1637,22 +1971,22 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21">
         <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" s="23">
+        <v>78</v>
+      </c>
+      <c r="L21" s="22">
         <v>41255</v>
       </c>
       <c r="U21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="6:22" x14ac:dyDescent="0.25">
@@ -1660,22 +1994,22 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J22">
         <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>86</v>
-      </c>
-      <c r="L22" s="23">
+        <v>79</v>
+      </c>
+      <c r="L22" s="22">
         <v>41255</v>
       </c>
       <c r="U22">
         <v>1</v>
       </c>
       <c r="V22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="6:22" x14ac:dyDescent="0.25">
@@ -1683,33 +2017,44 @@
         <v>2</v>
       </c>
       <c r="V23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F25" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="M25" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="26" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="20" t="s">
-        <v>59</v>
+      <c r="F26" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="K26" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="L26" t="s">
+        <v>144</v>
+      </c>
+      <c r="N26" t="s">
+        <v>140</v>
+      </c>
+      <c r="O26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="6:22" x14ac:dyDescent="0.25">
@@ -1725,6 +2070,15 @@
       <c r="K27">
         <v>1</v>
       </c>
+      <c r="L27" s="22">
+        <v>41255</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F28" s="7">
@@ -1738,6 +2092,15 @@
       </c>
       <c r="K28">
         <v>1</v>
+      </c>
+      <c r="L28" s="22">
+        <v>41255</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="6:22" x14ac:dyDescent="0.25">
@@ -1753,6 +2116,15 @@
       <c r="K29">
         <v>1</v>
       </c>
+      <c r="L29" s="22">
+        <v>41255</v>
+      </c>
+      <c r="N29">
+        <v>5</v>
+      </c>
+      <c r="O29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F30" s="7">
@@ -1766,6 +2138,9 @@
       </c>
       <c r="K30">
         <v>2</v>
+      </c>
+      <c r="L30" s="22">
+        <v>41255</v>
       </c>
     </row>
     <row r="31" spans="6:22" x14ac:dyDescent="0.25">
@@ -1781,138 +2156,416 @@
       <c r="K31">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L31" s="22">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="34" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F36" s="8">
         <v>1</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K36" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="L36" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="M36" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="N36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="O36" t="s">
+        <v>124</v>
+      </c>
+      <c r="P36" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>126</v>
+      </c>
+      <c r="R36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F37" s="10">
         <v>2</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="L37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>3000</v>
+      </c>
+      <c r="N37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F38" s="7">
         <v>3</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J38">
         <v>2</v>
       </c>
       <c r="K38" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="L38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F39" s="10">
         <v>4</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J39">
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="L39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F40" s="7">
         <v>5</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J40">
         <v>4</v>
       </c>
       <c r="K40" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L40">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="6:18" x14ac:dyDescent="0.25">
       <c r="J43" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="6:18" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
+        <v>87</v>
+      </c>
+      <c r="K44" t="s">
         <v>96</v>
       </c>
-      <c r="K44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>147</v>
+      </c>
+      <c r="M44" t="s">
+        <v>148</v>
+      </c>
+      <c r="N44" t="s">
+        <v>149</v>
+      </c>
+      <c r="O44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L45">
+        <v>10</v>
+      </c>
+      <c r="M45" s="28">
+        <v>4.8634259259259259E-2</v>
+      </c>
+      <c r="N45" s="22">
+        <v>41255</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46" t="s">
+        <v>121</v>
+      </c>
+      <c r="L46">
+        <v>12</v>
+      </c>
+      <c r="M46" s="28">
+        <v>4.8634259259259259E-2</v>
+      </c>
+      <c r="N46" s="22">
+        <v>41255</v>
+      </c>
+      <c r="O46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47" t="s">
+        <v>145</v>
+      </c>
+      <c r="L47">
+        <v>9</v>
+      </c>
+      <c r="M47" s="28">
+        <v>4.8634259259259259E-2</v>
+      </c>
+      <c r="N47" s="22">
+        <v>41255</v>
+      </c>
+      <c r="O47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s">
+        <v>146</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+      <c r="M48" s="28">
+        <v>4.8634259259259259E-2</v>
+      </c>
+      <c r="N48" s="22">
+        <v>41255</v>
+      </c>
+      <c r="O48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J53" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="10:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J54" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="K54" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="L54" t="s">
+        <v>115</v>
+      </c>
+      <c r="M54" t="s">
+        <v>116</v>
+      </c>
+      <c r="N54" t="s">
+        <v>117</v>
+      </c>
+      <c r="O54" t="s">
+        <v>118</v>
+      </c>
+      <c r="P54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>114</v>
+      </c>
+      <c r="L55" s="27">
+        <v>0.125</v>
+      </c>
+      <c r="M55" t="s">
+        <v>83</v>
+      </c>
+      <c r="N55" t="s">
+        <v>90</v>
+      </c>
+      <c r="O55" t="s">
+        <v>120</v>
+      </c>
+      <c r="P55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="56" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J62" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>129</v>
+      </c>
+      <c r="K63" t="s">
+        <v>130</v>
+      </c>
+      <c r="L63" t="s">
+        <v>131</v>
+      </c>
+      <c r="M63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>71</v>
+      </c>
+      <c r="L64" t="s">
+        <v>133</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65" t="s">
+        <v>135</v>
+      </c>
+      <c r="L65" t="s">
+        <v>133</v>
+      </c>
+      <c r="M65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D66" s="1"/>
+      <c r="J66">
+        <v>3</v>
+      </c>
+      <c r="K66" t="s">
+        <v>151</v>
+      </c>
+      <c r="L66" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J71" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>137</v>
+      </c>
+      <c r="K72" t="s">
+        <v>0</v>
+      </c>
+      <c r="L72" t="s">
+        <v>141</v>
+      </c>
+      <c r="M72" t="s">
+        <v>136</v>
+      </c>
+      <c r="N72" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <v>3</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <v>4</v>
+      </c>
+      <c r="K75">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +2576,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
-  <tableParts count="12">
+  <tableParts count="17">
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
@@ -1936,6 +2589,11 @@
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
     <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion de tablas artista, albunes
</commit_message>
<xml_diff>
--- a/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
+++ b/Modelo_de_base_de_datos/modelo Entidad-Relacion/Modelo Entidad- Relacion de spotify.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="179">
   <si>
     <t>Codigo usuario</t>
   </si>
@@ -326,48 +326,9 @@
     <t>Nombre de la cancion</t>
   </si>
   <si>
-    <t>Nombre de la ciudad</t>
-  </si>
-  <si>
-    <t>Codigo ciudad</t>
-  </si>
-  <si>
-    <t>codigo de codigo postal</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>Codigo departamento</t>
-  </si>
-  <si>
-    <t>Nombre del departamento</t>
-  </si>
-  <si>
     <t>Tegucigalpa</t>
   </si>
   <si>
-    <t>La Ceiba</t>
-  </si>
-  <si>
-    <t>Atlantida</t>
-  </si>
-  <si>
-    <t>dep. De guatemala</t>
-  </si>
-  <si>
-    <t>León</t>
-  </si>
-  <si>
-    <t>La Paz Centro</t>
-  </si>
-  <si>
-    <t>SAN PEDRO AYAMPUC</t>
-  </si>
-  <si>
     <t>No body can save me</t>
   </si>
   <si>
@@ -392,18 +353,9 @@
     <t>Give me all your luvin'</t>
   </si>
   <si>
-    <t>Segidores</t>
-  </si>
-  <si>
     <t>Biografia</t>
   </si>
   <si>
-    <t>Reportes recibidos</t>
-  </si>
-  <si>
-    <t>Numero de shares</t>
-  </si>
-  <si>
     <t>Conciertos</t>
   </si>
   <si>
@@ -480,13 +432,142 @@
   </si>
   <si>
     <t>hip hop</t>
+  </si>
+  <si>
+    <t>Fecha empezo a seguir</t>
+  </si>
+  <si>
+    <t>Codigo usuario X Codigo de grupo musical o artista</t>
+  </si>
+  <si>
+    <t>Fecha que reporto</t>
+  </si>
+  <si>
+    <t>Que reporta</t>
+  </si>
+  <si>
+    <t>Codigo de reporte</t>
+  </si>
+  <si>
+    <t>Cancion</t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Artista</t>
+  </si>
+  <si>
+    <t>Codigo que reporta</t>
+  </si>
+  <si>
+    <t>Codigo el que reporta</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Codigo que reporta can/alb/play/art</t>
+  </si>
+  <si>
+    <t>Codigo a que da share</t>
+  </si>
+  <si>
+    <t>A que da share</t>
+  </si>
+  <si>
+    <t>Codigo de Share</t>
+  </si>
+  <si>
+    <t>Codigo que share can/alb/play/art</t>
+  </si>
+  <si>
+    <t>Red social</t>
+  </si>
+  <si>
+    <t>Codigo de red social</t>
+  </si>
+  <si>
+    <t>Nombre de la red social</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twitter </t>
+  </si>
+  <si>
+    <t>Telegram</t>
+  </si>
+  <si>
+    <t>Skype</t>
+  </si>
+  <si>
+    <t>Tumblr</t>
+  </si>
+  <si>
+    <t>Codigo usuario X Codigo a que da share</t>
+  </si>
+  <si>
+    <t>Codigo usuario X Codigo el que reporta</t>
+  </si>
+  <si>
+    <t>Codigo concierto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha </t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>Tickes disponibles</t>
+  </si>
+  <si>
+    <t>Lugares</t>
+  </si>
+  <si>
+    <t>Codigo Lugar</t>
+  </si>
+  <si>
+    <t>Nombre Lugar</t>
+  </si>
+  <si>
+    <t>Codigo Lugar Padre</t>
+  </si>
+  <si>
+    <t>Codigo Tipo Lugar</t>
+  </si>
+  <si>
+    <t>CostaRica</t>
+  </si>
+  <si>
+    <t>Chiquimula</t>
+  </si>
+  <si>
+    <t>Intibuca</t>
+  </si>
+  <si>
+    <t>Algun municipio de chiquimula</t>
+  </si>
+  <si>
+    <t>La Esperanza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,13 +579,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -523,14 +597,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF005297"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,23 +608,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8F9FA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -683,51 +739,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA2A9B1"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFA2A9B1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA2A9B1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA2A9B1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -737,53 +754,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -819,7 +809,7 @@
   <tableColumns count="12">
     <tableColumn id="1" name="Codigo usuario"/>
     <tableColumn id="2" name="Nombre completo"/>
-    <tableColumn id="3" name="Fecha de nacimiento" dataDxfId="2"/>
+    <tableColumn id="3" name="Fecha de nacimiento" dataDxfId="0"/>
     <tableColumn id="4" name="Codigo Genero"/>
     <tableColumn id="5" name="Usuario de platafoma"/>
     <tableColumn id="6" name="Correo electonico"/>
@@ -835,34 +825,6 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="J36:R40" totalsRowShown="0">
-  <autoFilter ref="J36:R40">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Codigo de grupo musical o artista"/>
-    <tableColumn id="2" name="Nombre de grupo musical o artista"/>
-    <tableColumn id="3" name="codigo pais"/>
-    <tableColumn id="5" name="Segidores"/>
-    <tableColumn id="7" name="Biografia"/>
-    <tableColumn id="8" name="Reportes recibidos"/>
-    <tableColumn id="9" name="Numero de shares"/>
-    <tableColumn id="10" name="Conciertos"/>
-    <tableColumn id="11" name="Radio"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="J44:O48" totalsRowShown="0">
   <autoFilter ref="J44:O48">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -884,7 +846,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="J54:P57" totalsRowShown="0">
   <autoFilter ref="J54:P57">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -908,23 +870,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="Y12:AA16" totalsRowShown="0">
-  <autoFilter ref="Y12:AA16">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Codigo departamento"/>
-    <tableColumn id="2" name="Nombre del departamento"/>
-    <tableColumn id="3" name="Codigo pais"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="J63:M66" totalsRowShown="0">
   <autoFilter ref="J63:M66">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -942,7 +888,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="L72:N75" totalsRowShown="0">
   <autoFilter ref="L72:N75">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -958,7 +904,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="J72:K75" totalsRowShown="0">
   <autoFilter ref="J72:K75">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -972,7 +918,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="N26:O29" totalsRowShown="0">
   <autoFilter ref="N26:O29">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -981,6 +927,74 @@
   <tableColumns count="2">
     <tableColumn id="1" name="Codigo de genero musical"/>
     <tableColumn id="2" name="Codigo de grupo musical o artista"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="E46:G49" totalsRowShown="0">
+  <autoFilter ref="E46:G49">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Codigo usuario"/>
+    <tableColumn id="2" name="Codigo de grupo musical o artista"/>
+    <tableColumn id="3" name="Fecha empezo a seguir"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table19" displayName="Table19" ref="E55:H58" totalsRowShown="0">
+  <autoFilter ref="E55:H58">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Codigo usuario"/>
+    <tableColumn id="2" name="Codigo el que reporta"/>
+    <tableColumn id="3" name="Fecha que reporto"/>
+    <tableColumn id="4" name="Codigo que reporta can/alb/play/art"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="E63:F67" totalsRowShown="0">
+  <autoFilter ref="E63:F67">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo de reporte"/>
+    <tableColumn id="2" name="Que reporta"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table1922" displayName="Table1922" ref="J81:N84" totalsRowShown="0">
+  <autoFilter ref="J81:N84">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Codigo usuario"/>
+    <tableColumn id="2" name="Codigo a que da share"/>
+    <tableColumn id="3" name="Fecha que reporto"/>
+    <tableColumn id="4" name="Codigo que share can/alb/play/art"/>
+    <tableColumn id="5" name="Codigo de red social"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -995,6 +1009,54 @@
   <tableColumns count="2">
     <tableColumn id="1" name="Codigo Genero"/>
     <tableColumn id="2" name="Nombre Genero"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table2023" displayName="Table2023" ref="J89:K93" totalsRowShown="0">
+  <autoFilter ref="J89:K93">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo de Share"/>
+    <tableColumn id="2" name="A que da share"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table23" displayName="Table23" ref="M89:N94" totalsRowShown="0">
+  <autoFilter ref="M89:N94">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Codigo de red social"/>
+    <tableColumn id="2" name="Nombre de la red social"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="U27:Y30" totalsRowShown="0">
+  <autoFilter ref="U27:Y30">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Codigo concierto"/>
+    <tableColumn id="2" name="Codigo de grupo musical o artista"/>
+    <tableColumn id="3" name="Fecha "/>
+    <tableColumn id="4" name="pais"/>
+    <tableColumn id="5" name="Tickes disponibles"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1057,24 +1119,6 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="Y3:AB7" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="Y3:AB7">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Codigo ciudad"/>
-    <tableColumn id="2" name="Nombre de la ciudad"/>
-    <tableColumn id="3" name="codigo de codigo postal"/>
-    <tableColumn id="4" name="Codigo departamento"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="J12:L22" totalsRowShown="0">
   <autoFilter ref="J12:L22">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1090,7 +1134,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="J26:L31" totalsRowShown="0">
   <autoFilter ref="J26:L31">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1101,6 +1145,26 @@
     <tableColumn id="1" name="Codigo de genero musical"/>
     <tableColumn id="2" name="Codigo de usuario"/>
     <tableColumn id="3" name="Fecha en que anade genero a su cuenta"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="J36:N40" totalsRowShown="0">
+  <autoFilter ref="J36:N40">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Codigo de grupo musical o artista"/>
+    <tableColumn id="2" name="Nombre de grupo musical o artista"/>
+    <tableColumn id="3" name="codigo pais"/>
+    <tableColumn id="7" name="Biografia"/>
+    <tableColumn id="11" name="Radio"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AB75"/>
+  <dimension ref="B2:AD94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,12 +1444,12 @@
     <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41" customWidth="1"/>
+    <col min="10" max="10" width="50" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="41.5703125" customWidth="1"/>
     <col min="12" max="12" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="48.140625" bestFit="1" customWidth="1"/>
@@ -1395,15 +1459,17 @@
     <col min="18" max="18" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
     <col min="25" max="25" width="27.7109375" customWidth="1"/>
     <col min="26" max="26" width="32.42578125" customWidth="1"/>
     <col min="27" max="27" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.85546875" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1420,11 +1486,8 @@
       <c r="U2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="Y2" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1473,20 +1536,11 @@
       <c r="V3" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB3" s="26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1535,20 +1589,11 @@
       <c r="V4" t="s">
         <v>27</v>
       </c>
-      <c r="Y4" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA4" s="17">
-        <v>11101</v>
-      </c>
-      <c r="AB4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA4" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1597,20 +1642,20 @@
       <c r="V5" t="s">
         <v>94</v>
       </c>
-      <c r="Y5" s="20">
-        <v>2</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA5" s="18">
-        <v>31101</v>
-      </c>
-      <c r="AB5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA5" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD5" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -1653,48 +1698,82 @@
       <c r="V6" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" s="21">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA6" s="24">
-        <v>22100</v>
-      </c>
-      <c r="AB6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:28" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="AA6" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="U7">
         <v>4</v>
       </c>
       <c r="V7" t="s">
         <v>29</v>
       </c>
-      <c r="Y7" s="20">
-        <v>4</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA7" s="25">
-        <v>1056</v>
-      </c>
-      <c r="AB7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AA7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="U8">
         <v>5</v>
       </c>
       <c r="V8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AA8" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AA9" s="7">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AA10" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB10" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>32</v>
       </c>
@@ -1707,11 +1786,21 @@
       <c r="U11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="Y11" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y11" s="1"/>
+      <c r="AA11" s="7">
+        <v>6</v>
+      </c>
+      <c r="AB11" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -1725,13 +1814,13 @@
         <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="K12" t="s">
         <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="U12" s="12" t="s">
         <v>55</v>
@@ -1739,17 +1828,20 @@
       <c r="V12" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="Y12" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AA12" s="7">
+        <v>7</v>
+      </c>
+      <c r="AB12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC12" s="7">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1</v>
       </c>
@@ -1768,7 +1860,7 @@
       <c r="K13" t="s">
         <v>71</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="18">
         <v>41255</v>
       </c>
       <c r="U13" s="9">
@@ -1777,17 +1869,20 @@
       <c r="V13" s="9">
         <v>1</v>
       </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AA13" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC13" s="7">
+        <v>5</v>
+      </c>
+      <c r="AD13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2</v>
       </c>
@@ -1806,7 +1901,7 @@
       <c r="K14" t="s">
         <v>72</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="18">
         <v>41255</v>
       </c>
       <c r="U14" s="7">
@@ -1815,17 +1910,20 @@
       <c r="V14" s="7">
         <v>2</v>
       </c>
-      <c r="Y14">
-        <v>2</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AA14" s="7">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>6</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
@@ -1844,7 +1942,7 @@
       <c r="K15" t="s">
         <v>73</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="18">
         <v>41255</v>
       </c>
       <c r="U15" s="10">
@@ -1853,17 +1951,8 @@
       <c r="V15" s="10">
         <v>1</v>
       </c>
-      <c r="Y15">
-        <v>3</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>4</v>
       </c>
@@ -1876,7 +1965,7 @@
       <c r="K16" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="18">
         <v>41255</v>
       </c>
       <c r="U16" s="13">
@@ -1885,17 +1974,9 @@
       <c r="V16" s="13">
         <v>1</v>
       </c>
-      <c r="Y16">
-        <v>4</v>
-      </c>
-      <c r="Z16" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="Z16" s="19"/>
+    </row>
+    <row r="17" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>5</v>
       </c>
@@ -1908,11 +1989,11 @@
       <c r="K17" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="22">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="L17" s="18">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="18" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>6</v>
       </c>
@@ -1925,11 +2006,11 @@
       <c r="K18" t="s">
         <v>83</v>
       </c>
-      <c r="L18" s="22">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="L18" s="18">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="19" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>7</v>
       </c>
@@ -1942,11 +2023,11 @@
       <c r="K19" t="s">
         <v>76</v>
       </c>
-      <c r="L19" s="22">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="L19" s="18">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="20" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>8</v>
       </c>
@@ -1959,14 +2040,14 @@
       <c r="K20" t="s">
         <v>77</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="18">
         <v>41255</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>9</v>
       </c>
@@ -1979,7 +2060,7 @@
       <c r="K21" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="22">
+      <c r="L21" s="18">
         <v>41255</v>
       </c>
       <c r="U21" t="s">
@@ -1989,7 +2070,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>10</v>
       </c>
@@ -2002,7 +2083,7 @@
       <c r="K22" t="s">
         <v>79</v>
       </c>
-      <c r="L22" s="22">
+      <c r="L22" s="18">
         <v>41255</v>
       </c>
       <c r="U22">
@@ -2012,7 +2093,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:25" x14ac:dyDescent="0.25">
       <c r="U23">
         <v>2</v>
       </c>
@@ -2020,7 +2101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F25" s="7" t="s">
         <v>64</v>
       </c>
@@ -2031,33 +2112,36 @@
         <v>81</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="6:25" x14ac:dyDescent="0.25">
+      <c r="F26" s="17" t="s">
         <v>58</v>
       </c>
       <c r="G26" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="K26" t="s">
         <v>82</v>
       </c>
       <c r="L26" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="N26" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="O26" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U26" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F27" s="10">
         <v>1</v>
       </c>
@@ -2070,7 +2154,7 @@
       <c r="K27">
         <v>1</v>
       </c>
-      <c r="L27" s="22">
+      <c r="L27" s="18">
         <v>41255</v>
       </c>
       <c r="N27">
@@ -2079,8 +2163,23 @@
       <c r="O27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
+        <v>165</v>
+      </c>
+      <c r="V27" t="s">
+        <v>86</v>
+      </c>
+      <c r="W27" t="s">
+        <v>166</v>
+      </c>
+      <c r="X27" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F28" s="7">
         <v>1</v>
       </c>
@@ -2093,7 +2192,7 @@
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="L28" s="22">
+      <c r="L28" s="18">
         <v>41255</v>
       </c>
       <c r="N28">
@@ -2102,8 +2201,23 @@
       <c r="O28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28" s="18">
+        <v>41255</v>
+      </c>
+      <c r="X28">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="29" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F29" s="10">
         <v>3</v>
       </c>
@@ -2116,7 +2230,7 @@
       <c r="K29">
         <v>1</v>
       </c>
-      <c r="L29" s="22">
+      <c r="L29" s="18">
         <v>41255</v>
       </c>
       <c r="N29">
@@ -2125,8 +2239,23 @@
       <c r="O29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>3</v>
+      </c>
+      <c r="W29" s="18">
+        <v>41255</v>
+      </c>
+      <c r="X29">
+        <v>5</v>
+      </c>
+      <c r="Y29">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F30" s="7">
         <v>2</v>
       </c>
@@ -2139,11 +2268,26 @@
       <c r="K30">
         <v>2</v>
       </c>
-      <c r="L30" s="22">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="31" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="L30" s="18">
+        <v>41255</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+      <c r="V30">
+        <v>4</v>
+      </c>
+      <c r="W30" s="18">
+        <v>41255</v>
+      </c>
+      <c r="X30">
+        <v>5</v>
+      </c>
+      <c r="Y30">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="31" spans="6:25" x14ac:dyDescent="0.25">
       <c r="F31" s="10">
         <v>4</v>
       </c>
@@ -2156,16 +2300,16 @@
       <c r="K31">
         <v>3</v>
       </c>
-      <c r="L31" s="22">
-        <v>41255</v>
-      </c>
-    </row>
-    <row r="34" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L31" s="18">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="14" t="s">
         <v>58</v>
       </c>
@@ -2176,7 +2320,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F36" s="8">
         <v>1</v>
       </c>
@@ -2193,25 +2337,13 @@
         <v>88</v>
       </c>
       <c r="M36" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="N36" t="s">
-        <v>123</v>
-      </c>
-      <c r="O36" t="s">
-        <v>124</v>
-      </c>
-      <c r="P36" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>126</v>
-      </c>
-      <c r="R36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="6:18" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F37" s="10">
         <v>2</v>
       </c>
@@ -2227,14 +2359,11 @@
       <c r="L37">
         <v>5</v>
       </c>
-      <c r="M37">
-        <v>3000</v>
-      </c>
-      <c r="N37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F38" s="7">
         <v>3</v>
       </c>
@@ -2250,11 +2379,11 @@
       <c r="L38">
         <v>5</v>
       </c>
-      <c r="N38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F39" s="10">
         <v>4</v>
       </c>
@@ -2270,11 +2399,11 @@
       <c r="L39">
         <v>1</v>
       </c>
-      <c r="N39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F40" s="7">
         <v>5</v>
       </c>
@@ -2290,16 +2419,16 @@
       <c r="L40">
         <v>2</v>
       </c>
-      <c r="N40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.25">
       <c r="J43" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:15" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
         <v>87</v>
       </c>
@@ -2307,104 +2436,148 @@
         <v>96</v>
       </c>
       <c r="L44" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="M44" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="N44" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="O44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E45" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="J45">
         <v>1</v>
       </c>
       <c r="K45" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="L45">
         <v>10</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M45" s="21">
         <v>4.8634259259259259E-2</v>
       </c>
-      <c r="N45" s="22">
+      <c r="N45" s="18">
         <v>41255</v>
       </c>
       <c r="O45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>86</v>
+      </c>
+      <c r="G46" t="s">
+        <v>136</v>
+      </c>
       <c r="J46">
         <v>2</v>
       </c>
       <c r="K46" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="L46">
         <v>12</v>
       </c>
-      <c r="M46" s="28">
+      <c r="M46" s="21">
         <v>4.8634259259259259E-2</v>
       </c>
-      <c r="N46" s="22">
+      <c r="N46" s="18">
         <v>41255</v>
       </c>
       <c r="O46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" s="18">
+        <v>41255</v>
+      </c>
       <c r="J47">
         <v>3</v>
       </c>
       <c r="K47" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="L47">
         <v>9</v>
       </c>
-      <c r="M47" s="28">
+      <c r="M47" s="21">
         <v>4.8634259259259259E-2</v>
       </c>
-      <c r="N47" s="22">
+      <c r="N47" s="18">
         <v>41255</v>
       </c>
       <c r="O47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48" s="18">
+        <v>41255</v>
+      </c>
       <c r="J48">
         <v>4</v>
       </c>
       <c r="K48" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="L48">
         <v>5</v>
       </c>
-      <c r="M48" s="28">
+      <c r="M48" s="21">
         <v>4.8634259259259259E-2</v>
       </c>
-      <c r="N48" s="22">
+      <c r="N48" s="18">
         <v>41255</v>
       </c>
       <c r="O48">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" s="18">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="53" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J53" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E54" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="J54" t="s">
         <v>98</v>
       </c>
@@ -2412,29 +2585,41 @@
         <v>99</v>
       </c>
       <c r="L54" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="M54" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="N54" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="O54" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="P54" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="10:16" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>145</v>
+      </c>
+      <c r="G55" t="s">
+        <v>138</v>
+      </c>
+      <c r="H55" t="s">
+        <v>150</v>
+      </c>
       <c r="J55">
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>114</v>
-      </c>
-      <c r="L55" s="27">
+        <v>101</v>
+      </c>
+      <c r="L55" s="20">
         <v>0.125</v>
       </c>
       <c r="M55" t="s">
@@ -2444,42 +2629,95 @@
         <v>90</v>
       </c>
       <c r="O55" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="P55">
         <v>5000</v>
       </c>
     </row>
-    <row r="56" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56" s="18">
+        <v>41255</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
       <c r="J56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57" s="18">
+        <v>41255</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
       <c r="J57">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="10:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58" s="18">
+        <v>41255</v>
+      </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E62" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="J62" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" spans="10:16" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>140</v>
+      </c>
+      <c r="F63" t="s">
+        <v>139</v>
+      </c>
       <c r="J63" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="K63" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="L63" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="M63" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="10:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>141</v>
+      </c>
       <c r="J64">
         <v>1</v>
       </c>
@@ -2487,21 +2725,27 @@
         <v>71</v>
       </c>
       <c r="L64" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="M64">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s">
+        <v>142</v>
+      </c>
       <c r="J65">
         <v>2</v>
       </c>
       <c r="K65" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="L65" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="M65">
         <v>2</v>
@@ -2509,14 +2753,28 @@
     </row>
     <row r="66" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="s">
+        <v>143</v>
+      </c>
       <c r="J66">
         <v>3</v>
       </c>
       <c r="K66" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="L66" t="s">
-        <v>134</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="4:14" x14ac:dyDescent="0.25">
@@ -2524,24 +2782,24 @@
     </row>
     <row r="71" spans="4:14" x14ac:dyDescent="0.25">
       <c r="J71" s="7" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="4:14" x14ac:dyDescent="0.25">
       <c r="J72" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="K72" t="s">
         <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="M72" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="N72" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="4:14" x14ac:dyDescent="0.25">
@@ -2566,6 +2824,165 @@
       </c>
       <c r="K75">
         <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J80" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>0</v>
+      </c>
+      <c r="K81" t="s">
+        <v>151</v>
+      </c>
+      <c r="L81" t="s">
+        <v>138</v>
+      </c>
+      <c r="M81" t="s">
+        <v>154</v>
+      </c>
+      <c r="N81" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="K82">
+        <v>3</v>
+      </c>
+      <c r="L82" s="18">
+        <v>41255</v>
+      </c>
+      <c r="M82">
+        <v>1</v>
+      </c>
+      <c r="N82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="K83">
+        <v>2</v>
+      </c>
+      <c r="L83" s="18">
+        <v>41255</v>
+      </c>
+      <c r="M83">
+        <v>3</v>
+      </c>
+      <c r="N83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <v>2</v>
+      </c>
+      <c r="K84">
+        <v>4</v>
+      </c>
+      <c r="L84" s="18">
+        <v>41255</v>
+      </c>
+      <c r="M84">
+        <v>4</v>
+      </c>
+      <c r="N84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J88" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="M88" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>153</v>
+      </c>
+      <c r="K89" t="s">
+        <v>152</v>
+      </c>
+      <c r="M89" t="s">
+        <v>156</v>
+      </c>
+      <c r="N89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="K90" t="s">
+        <v>141</v>
+      </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+      <c r="N90" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <v>2</v>
+      </c>
+      <c r="K91" t="s">
+        <v>142</v>
+      </c>
+      <c r="M91">
+        <v>2</v>
+      </c>
+      <c r="N91" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <v>3</v>
+      </c>
+      <c r="K92" t="s">
+        <v>143</v>
+      </c>
+      <c r="M92">
+        <v>3</v>
+      </c>
+      <c r="N92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <v>4</v>
+      </c>
+      <c r="K93" t="s">
+        <v>111</v>
+      </c>
+      <c r="M93">
+        <v>4</v>
+      </c>
+      <c r="N93" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="94" spans="10:14" x14ac:dyDescent="0.25">
+      <c r="M94">
+        <v>5</v>
+      </c>
+      <c r="N94" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2576,7 +2993,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
-  <tableParts count="17">
+  <tableParts count="22">
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
@@ -2594,6 +3011,11 @@
     <tablePart r:id="rId19"/>
     <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId26"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>